<commit_message>
Updated Analysis with AIC
</commit_message>
<xml_diff>
--- a/datafiles/ModelFit.xlsx
+++ b/datafiles/ModelFit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/triciavanlaar/Desktop/CSUStan/Research/Manuscripts/Biehleretal/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{438AAA3C-3CE7-2D44-802E-8F459F0DA1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C4E1BB-052A-B444-9D4F-AA2FCB016E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17960" yWindow="820" windowWidth="28040" windowHeight="17240" xr2:uid="{F3B62104-4846-F943-9E20-1F702429CD56}"/>
+    <workbookView xWindow="43600" yWindow="3520" windowWidth="28040" windowHeight="17240" xr2:uid="{F3B62104-4846-F943-9E20-1F702429CD56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Model</t>
   </si>
@@ -50,43 +50,16 @@
     <t>Log Likelihood</t>
   </si>
   <si>
-    <t>Species + Sex + Year + Season</t>
-  </si>
-  <si>
-    <t>Species + Season</t>
-  </si>
-  <si>
-    <t>Species + Year</t>
-  </si>
-  <si>
-    <t>Species + Sex * Season + Year</t>
-  </si>
-  <si>
-    <t>Species + Season + Year</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
-    <t>Species * Sex + Year</t>
-  </si>
-  <si>
-    <t>Species * Sex + Season</t>
-  </si>
-  <si>
-    <t>Species + Sex * Season</t>
-  </si>
-  <si>
-    <t>Species + Sex * Year</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Season</t>
+    <t>Species + Sex</t>
+  </si>
+  <si>
+    <t>Species * Sex</t>
   </si>
 </sst>
 </file>
@@ -478,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6051ED1-15FC-D348-B13E-CEEAB762C851}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,16 +480,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>-563.4</v>
+        <v>-553.6</v>
       </c>
       <c r="C2" s="3">
-        <v>0.87260000000000004</v>
+        <v>0.86180000000000001</v>
       </c>
       <c r="D2" s="2">
-        <v>289.7</v>
+        <v>281.8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -524,172 +497,46 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>-561.70000000000005</v>
+        <v>-549.70000000000005</v>
       </c>
       <c r="C3" s="3">
-        <v>0.87</v>
+        <v>0.86250000000000004</v>
       </c>
       <c r="D3" s="2">
-        <v>287.89999999999998</v>
+        <v>280.8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>-559.79999999999995</v>
+        <v>-545.1</v>
       </c>
       <c r="C4" s="3">
-        <v>0.87350000000000005</v>
+        <v>0.86350000000000005</v>
       </c>
       <c r="D4" s="2">
-        <v>288.89999999999998</v>
+        <v>281.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>-559.70000000000005</v>
+        <v>-160.9</v>
       </c>
       <c r="C5" s="3">
-        <v>0.87480000000000002</v>
+        <v>1.41E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>289.89999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>-558</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.87370000000000003</v>
-      </c>
-      <c r="D6" s="2">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-554.1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.86370000000000002</v>
-      </c>
-      <c r="D7" s="2">
-        <v>283.10000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-553.6</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.86180000000000001</v>
-      </c>
-      <c r="D8" s="2">
-        <v>281.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
-        <v>-553.1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.87160000000000004</v>
-      </c>
-      <c r="D9" s="2">
-        <v>287.60000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-548.4</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.86460000000000004</v>
-      </c>
-      <c r="D10" s="2">
-        <v>282.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-544.9</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.86499999999999999</v>
-      </c>
-      <c r="D11" s="2">
-        <v>282.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>-432</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.74950000000000006</v>
-      </c>
-      <c r="D12" s="2">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-293.2</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="D13" s="2">
-        <v>150.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
-        <v>-160.9</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.41E-2</v>
-      </c>
-      <c r="D14" s="2">
         <v>83.4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D14">
-    <sortCondition ref="B2:B14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D5">
+    <sortCondition ref="B2:B5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>